<commit_message>
Add navigation links to templates and enhance UI with improved styles
</commit_message>
<xml_diff>
--- a/static/files/Credits and Debits Expen.xlsx
+++ b/static/files/Credits and Debits Expen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MADHAV SAI ARYAN\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MADHAV SAI ARYAN\Documents\ExpenaPP\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45C195E8-7DA1-4D4A-B786-F50942395006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828658E8-6F5B-4AEE-BDDA-EE3472FF8FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E5B0B2B8-E38D-4673-84F6-7CF211328A20}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12504" activeTab="1" xr2:uid="{E5B0B2B8-E38D-4673-84F6-7CF211328A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Credits" sheetId="1" r:id="rId1"/>
@@ -59,15 +59,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>eric</t>
-  </si>
-  <si>
-    <t>nelson</t>
   </si>
   <si>
     <t>Name/Namn</t>
@@ -99,6 +93,15 @@
   <si>
     <t>Date / Datum</t>
   </si>
+  <si>
+    <t>madhav</t>
+  </si>
+  <si>
+    <t>sai</t>
+  </si>
+  <si>
+    <t>aryan</t>
+  </si>
 </sst>
 </file>
 
@@ -106,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -142,12 +145,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -168,9 +171,6 @@
       <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -180,10 +180,13 @@
       <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -209,13 +212,13 @@
     <tableColumn id="2" xr3:uid="{00898C11-2016-4575-A20E-5CD6E2C6758E}" name="Date/ Datum" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{CC4BCBFE-BD08-4BD6-9B8B-8055229A8F1D}" name="Start time/ Starttid" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{7CAFF184-08EA-4250-AF9B-4BFB0B1445D1}" name="End time/ Sluttid" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{F853D63F-C26B-4799-AF3E-B5C614CAAA58}" name="Amount made/ Intjänat belopp" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{F853D63F-C26B-4799-AF3E-B5C614CAAA58}" name="Amount made/ Intjänat belopp" dataDxfId="5">
       <calculatedColumnFormula xml:space="preserve"> G2 * 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F79D9552-16B4-41D8-9ED4-3F388A62BD76}" name="balance / Saldo" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{F79D9552-16B4-41D8-9ED4-3F388A62BD76}" name="balance / Saldo" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(SUMIFS(E$2:E2, A$2:A2, A2) - SUMIFS(Debits!C:C, Debits!A:A, A2, Debits!B:B, "&lt;=" &amp; B2), E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{99165286-BA39-4AE7-B60A-D63BDF739D6D}" name="Duration /  Varaktighet" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{99165286-BA39-4AE7-B60A-D63BDF739D6D}" name="Duration /  Varaktighet" dataDxfId="3">
       <calculatedColumnFormula xml:space="preserve"> (HOUR(D2) + MINUTE(D2)/60 + SECOND(D2)/3600) - (HOUR(C2) + MINUTE(C2)/60 + SECOND(C2)/3600)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -228,9 +231,9 @@
   <autoFilter ref="A1:D31" xr:uid="{95717187-213F-43D5-A03E-FE8D52709493}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{89EE85BC-5A6C-454B-86AF-1307004C86F1}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{0AD07831-5232-444A-BF5A-EE731BC0D295}" name="Date / Datum" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{75C8D8E0-7A30-4C8F-B05D-14F5528EE6E7}" name="Amount spent/ Spenderat belopp" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C85D1B3F-056B-410C-BFAF-68491940B958}" name="Balance / Saldo" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{0AD07831-5232-444A-BF5A-EE731BC0D295}" name="Date / Datum" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{75C8D8E0-7A30-4C8F-B05D-14F5528EE6E7}" name="Amount spent/ Spenderat belopp" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C85D1B3F-056B-410C-BFAF-68491940B958}" name="Balance / Saldo" dataDxfId="0">
       <calculatedColumnFormula array="1">IFERROR(INDEX(Credits!F:F, MATCH(A2 &amp; _xlfn.MAXIFS(Credits!B:B, Credits!A:A, A2, Credits!B:B, "&lt;=" &amp; B2), Credits!A:A &amp; Credits!B:B, 0)) - SUMIF(A$2:A2, A2, C$2:C2), -C2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -557,9 +560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC128B1-BBC2-495F-B127-DE3B9D9D04DE}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,30 +578,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>45573</v>
@@ -610,7 +613,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E2" s="5">
-        <f xml:space="preserve"> G2 * 20</f>
+        <f t="shared" ref="E2:E9" si="0" xml:space="preserve"> G2 * 20</f>
         <v>30</v>
       </c>
       <c r="F2" s="5">
@@ -624,7 +627,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>45574</v>
@@ -636,7 +639,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E3" s="5">
-        <f xml:space="preserve"> G3 * 20</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="F3" s="5">
@@ -644,13 +647,13 @@
         <v>60</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G33" si="0" xml:space="preserve"> (HOUR(D3) + MINUTE(D3)/60 + SECOND(D3)/3600) - (HOUR(C3) + MINUTE(C3)/60 + SECOND(C3)/3600)</f>
+        <f t="shared" ref="G3:G33" si="1" xml:space="preserve"> (HOUR(D3) + MINUTE(D3)/60 + SECOND(D3)/3600) - (HOUR(C3) + MINUTE(C3)/60 + SECOND(C3)/3600)</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>45575</v>
@@ -662,21 +665,21 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E4" s="5">
-        <f xml:space="preserve"> G4 * 20</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="F4" s="5">
         <f>IFERROR(SUMIFS(E$2:E4, A$2:A4, A4) - SUMIFS(Debits!C:C, Debits!A:A, A4, Debits!B:B, "&lt;=" &amp; B4), E4)</f>
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>45576</v>
@@ -688,7 +691,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E5" s="5">
-        <f xml:space="preserve"> G5 * 20</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="F5" s="5">
@@ -696,13 +699,13 @@
         <v>105</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>45577</v>
@@ -714,21 +717,21 @@
         <v>0.625</v>
       </c>
       <c r="E6" s="5">
-        <f xml:space="preserve"> G6 * 20</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F6" s="5">
         <f>IFERROR(SUMIFS(E$2:E6, A$2:A6, A6) - SUMIFS(Debits!C:C, Debits!A:A, A6, Debits!B:B, "&lt;=" &amp; B6), E6)</f>
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>45578</v>
@@ -740,31 +743,34 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E7" s="5">
-        <f xml:space="preserve"> G7 * 20</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F7" s="5">
         <f>IFERROR(SUMIFS(E$2:E7, A$2:A7, A7) - SUMIFS(Debits!C:C, Debits!A:A, A7, Debits!B:B, "&lt;=" &amp; B7), E7)</f>
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="E8" s="5">
-        <f xml:space="preserve"> G8 * 20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="5">
         <f>IFERROR(SUMIFS(E$2:E8, A$2:A8, A8) - SUMIFS(Debits!C:C, Debits!A:A, A8, Debits!B:B, "&lt;=" &amp; B8), E8)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -772,7 +778,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="E9" s="5">
-        <f xml:space="preserve"> G9 * 20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="5">
@@ -780,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -788,7 +794,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="4"/>
       <c r="E10" s="5">
-        <f t="shared" ref="E10:E33" si="1" xml:space="preserve"> G10 * 20</f>
+        <f t="shared" ref="E10:E33" si="2" xml:space="preserve"> G10 * 20</f>
         <v>0</v>
       </c>
       <c r="F10" s="5">
@@ -796,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -804,7 +810,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="4"/>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F11" s="5">
@@ -812,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -820,7 +826,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="4"/>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F12" s="5">
@@ -828,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -836,7 +842,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="4"/>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13" s="5">
@@ -844,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -852,7 +858,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="4"/>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F14" s="5">
@@ -860,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -868,7 +874,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="4"/>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F15" s="5">
@@ -876,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -884,7 +890,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="4"/>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F16" s="5">
@@ -892,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -900,7 +906,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="4"/>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F17" s="5">
@@ -908,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -916,7 +922,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="4"/>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18" s="5">
@@ -924,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -932,7 +938,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="4"/>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F19" s="5">
@@ -940,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -948,7 +954,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="4"/>
       <c r="E20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F20" s="5">
@@ -956,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -964,7 +970,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="4"/>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F21" s="5">
@@ -972,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -980,7 +986,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="4"/>
       <c r="E22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F22" s="5">
@@ -988,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -996,7 +1002,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="4"/>
       <c r="E23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F23" s="5">
@@ -1004,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1012,7 +1018,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="4"/>
       <c r="E24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F24" s="5">
@@ -1020,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1028,7 +1034,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="4"/>
       <c r="E25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F25" s="5">
@@ -1036,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1044,7 +1050,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="4"/>
       <c r="E26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F26" s="5">
@@ -1052,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1060,7 +1066,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="4"/>
       <c r="E27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F27" s="5">
@@ -1068,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1076,7 +1082,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="4"/>
       <c r="E28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F28" s="5">
@@ -1084,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1092,7 +1098,7 @@
       <c r="B29" s="1"/>
       <c r="C29" s="4"/>
       <c r="E29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F29" s="5">
@@ -1100,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1108,7 +1114,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
       <c r="E30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F30" s="5">
@@ -1116,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1124,7 +1130,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
       <c r="E31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F31" s="5">
@@ -1132,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1140,7 +1146,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="4"/>
       <c r="E32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F32" s="5">
@@ -1148,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1156,7 +1162,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="4"/>
       <c r="E33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F33" s="5">
@@ -1164,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1196,14 +1202,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405CA5DF-76E2-4949-A89C-4AF43F0AA212}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" style="5" customWidth="1"/>
@@ -1214,18 +1220,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>45574</v>
@@ -1244,7 +1250,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>45575</v>
@@ -1259,7 +1265,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>45576</v>
@@ -1269,12 +1275,12 @@
       </c>
       <c r="D4" s="5" cm="1">
         <f t="array" ref="D4">IFERROR(INDEX(Credits!F:F, MATCH(A4 &amp; _xlfn.MAXIFS(Credits!B:B, Credits!A:A, A4, Credits!B:B, "&lt;=" &amp; B4), Credits!A:A &amp; Credits!B:B, 0)) - SUMIF(A$2:A4, A4, C$2:C4), -C4)</f>
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>45577</v>
@@ -1289,7 +1295,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>45579</v>
@@ -1299,13 +1305,22 @@
       </c>
       <c r="D6" s="5" cm="1">
         <f t="array" ref="D6">IFERROR(INDEX(Credits!F:F, MATCH(A6 &amp; _xlfn.MAXIFS(Credits!B:B, Credits!A:A, A6, Credits!B:B, "&lt;=" &amp; B6), Credits!A:A &amp; Credits!B:B, 0)) - SUMIF(A$2:A6, A6, C$2:C6), -C6)</f>
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45580</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
       <c r="D7" s="5" cm="1">
         <f t="array" ref="D7">IFERROR(INDEX(Credits!F:F, MATCH(A7 &amp; _xlfn.MAXIFS(Credits!B:B, Credits!A:A, A7, Credits!B:B, "&lt;=" &amp; B7), Credits!A:A &amp; Credits!B:B, 0)) - SUMIF(A$2:A7, A7, C$2:C7), -C7)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>